<commit_message>
Wrote the code to generate phase2 outcomes
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc.sharepoint.com/sites/EPISafe2Treat/Shared Documents/Projects/Simulation_Chase/Right censoring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{A4E19042-E281-6947-A6D3-DBDDCF0E8CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B091A0-2F07-F44F-8B79-595DBBD3B056}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB50349B-7940-B24B-B465-024B1710078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="560" windowWidth="28040" windowHeight="16180" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -89,6 +89,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={2761945B-CCCA-C740-B794-13037E1324C6}</author>
+    <author>tc={642DC8BF-9352-A841-B7D5-D2353D7406FD}</author>
     <author>tc={4C6D7E70-155D-F143-8348-12998FB8F68A}</author>
     <author>tc={0750D8B8-3F43-0249-A235-DC6D645DAACD}</author>
     <author>tc={2685FFE7-F524-DD45-9B6C-36B63629A0C0}</author>
@@ -104,7 +105,15 @@
     Decreased risk of fetal death at each gestational week (0.8*). However, didn’t change the probabilities of live birth.</t>
       </text>
     </comment>
-    <comment ref="C17" authorId="1" shapeId="0" xr:uid="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{642DC8BF-9352-A841-B7D5-D2353D7406FD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Values for gw 0-4 are the same because people wouldn’t actually be treated at this point, even if they entered the trial. This will be dealt with on the coding side.</t>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="2" shapeId="0" xr:uid="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -112,7 +121,7 @@
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
       </text>
     </comment>
-    <comment ref="D22" authorId="2" shapeId="0" xr:uid="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
+    <comment ref="D26" authorId="3" shapeId="0" xr:uid="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -120,7 +129,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
       </text>
     </comment>
-    <comment ref="C33" authorId="3" shapeId="0" xr:uid="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
+    <comment ref="C37" authorId="4" shapeId="0" xr:uid="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -270,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -358,24 +367,21 @@
   <si>
     <t>gestweek_conception</t>
   </si>
+  <si>
+    <t>p_index</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -421,14 +427,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,13 +778,16 @@
   <threadedComment ref="C1" dT="2023-10-27T16:14:10.42" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{B5EC156C-05C8-9940-B248-B21CC12432F7}" parentId="{2761945B-CCCA-C740-B794-13037E1324C6}">
     <text>Decreased risk of fetal death at each gestational week (0.8*). However, didn’t change the probabilities of live birth.</text>
   </threadedComment>
-  <threadedComment ref="C17" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
+  <threadedComment ref="A2" dT="2023-11-25T18:21:45.43" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{642DC8BF-9352-A841-B7D5-D2353D7406FD}">
+    <text>Values for gw 0-4 are the same because people wouldn’t actually be treated at this point, even if they entered the trial. This will be dealt with on the coding side.</text>
+  </threadedComment>
+  <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
-  <threadedComment ref="D22" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
+  <threadedComment ref="D26" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</text>
   </threadedComment>
-  <threadedComment ref="C33" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
+  <threadedComment ref="C37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</text>
   </threadedComment>
 </ThreadedComments>
@@ -845,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +868,7 @@
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -872,8 +881,11 @@
       <c r="D1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -887,8 +899,11 @@
         <f>1-C2-B2</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -902,8 +917,11 @@
         <f t="shared" ref="D3:D6" si="0">1-C3-B3</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -917,8 +935,11 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -932,8 +953,11 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -947,8 +971,11 @@
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -959,11 +986,14 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>1-B7-C7</f>
+        <f t="shared" ref="D7:D41" si="1">1-B7-C7</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -974,11 +1004,14 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>1-B8-C8</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -989,11 +1022,14 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>1-B9-C9</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1004,11 +1040,14 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>1-B10-C10</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1019,11 +1058,14 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>1-B11-C11</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1034,11 +1076,14 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>1-B12-C12</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1049,11 +1094,14 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>1-B13-C13</f>
+        <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1064,11 +1112,14 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>1-B14-C14</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1079,11 +1130,14 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f>1-B15-C15</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1094,11 +1148,14 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>1-B16-C16</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1109,11 +1166,14 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>1-B17-C17</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1124,11 +1184,14 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f>1-B18-C18</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1139,11 +1202,14 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f>1-B19-C19</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1154,11 +1220,14 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <f>1-B20-C20</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1169,11 +1238,14 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f>1-B21-C21</f>
+        <f t="shared" si="1"/>
         <v>0.997</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1184,11 +1256,14 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <f>1-B22-C22</f>
+        <f t="shared" si="1"/>
         <v>0.997</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1199,11 +1274,14 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <f>1-B23-C23</f>
+        <f t="shared" si="1"/>
         <v>0.997</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1214,11 +1292,14 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f>1-B24-C24</f>
+        <f t="shared" si="1"/>
         <v>0.997</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1229,11 +1310,14 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f>1-B25-C25</f>
+        <f t="shared" si="1"/>
         <v>0.997</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1244,11 +1328,14 @@
         <v>0.01</v>
       </c>
       <c r="D26">
-        <f>1-B26-C26</f>
+        <f t="shared" si="1"/>
         <v>0.98699999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1259,11 +1346,14 @@
         <v>0.01</v>
       </c>
       <c r="D27">
-        <f>1-B27-C27</f>
+        <f t="shared" si="1"/>
         <v>0.98699999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1274,11 +1364,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D28">
-        <f>1-B28-C28</f>
+        <f t="shared" si="1"/>
         <v>0.98199999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1289,11 +1382,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29">
-        <f>1-B29-C29</f>
+        <f t="shared" si="1"/>
         <v>0.98199999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1304,11 +1400,14 @@
         <v>0.02</v>
       </c>
       <c r="D30">
-        <f>1-B30-C30</f>
+        <f t="shared" si="1"/>
         <v>0.97699999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1319,11 +1418,14 @@
         <v>0.02</v>
       </c>
       <c r="D31">
-        <f>1-B31-C31</f>
+        <f t="shared" si="1"/>
         <v>0.97699999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1334,11 +1436,14 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D32">
-        <f>1-B32-C32</f>
+        <f t="shared" si="1"/>
         <v>0.97199999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1349,11 +1454,14 @@
         <v>0.03</v>
       </c>
       <c r="D33">
-        <f>1-B33-C33</f>
+        <f t="shared" si="1"/>
         <v>0.96699999999999997</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1364,11 +1472,14 @@
         <v>0.09</v>
       </c>
       <c r="D34">
-        <f>1-B34-C34</f>
+        <f t="shared" si="1"/>
         <v>0.90700000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1379,11 +1490,14 @@
         <v>0.09</v>
       </c>
       <c r="D35">
-        <f>1-B35-C35</f>
+        <f t="shared" si="1"/>
         <v>0.90700000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1394,11 +1508,14 @@
         <v>0.09</v>
       </c>
       <c r="D36">
-        <f>1-B36-C36</f>
+        <f t="shared" si="1"/>
         <v>0.90700000000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1410,11 +1527,14 @@
         <v>0.3</v>
       </c>
       <c r="D37">
-        <f>1-B37-C37</f>
+        <f t="shared" si="1"/>
         <v>0.69978999999999991</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1425,11 +1545,14 @@
         <v>0.35</v>
       </c>
       <c r="D38">
-        <f>1-B38-C38</f>
+        <f t="shared" si="1"/>
         <v>0.64973000000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1440,11 +1563,14 @@
         <v>0.7</v>
       </c>
       <c r="D39">
-        <f>1-B39-C39</f>
+        <f t="shared" si="1"/>
         <v>0.29965000000000008</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1455,11 +1581,14 @@
         <v>0.7</v>
       </c>
       <c r="D40">
-        <f>1-B40-C40</f>
+        <f t="shared" si="1"/>
         <v>0.29958000000000007</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1470,11 +1599,14 @@
         <v>0.7</v>
       </c>
       <c r="D41">
-        <f>1-B41-C41</f>
+        <f t="shared" si="1"/>
         <v>0.29939000000000004</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1486,6 +1618,9 @@
         <v>0.99892000000000003</v>
       </c>
       <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
         <v>0</v>
       </c>
     </row>
@@ -1497,18 +1632,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1519,715 +1655,787 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>1-D2-C2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="0">1-D3-C3</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <f>0.8*Phase1!B6</f>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2" si="0">1-D2-C2</f>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6" si="1">1-D6-C6</f>
         <v>0.96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <f>0.8*Phase1!B7</f>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>1-C3-D3</f>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E41" si="2">1-C7-D7</f>
         <v>0.96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C8">
         <f>0.8*Phase1!B8</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f>1-C4-D4</f>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C9">
         <f>0.8*Phase1!B9</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>1-C5-D5</f>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C10">
         <f>0.8*Phase1!B10</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>1-C6-D6</f>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C11">
         <f>0.8*Phase1!B11</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f>1-C7-D7</f>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C12">
         <f>0.8*Phase1!B12</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>1-C8-D8</f>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C13">
         <f>0.8*Phase1!B13</f>
         <v>2.4E-2</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>1-C9-D9</f>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C14">
         <f>0.8*Phase1!B14</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>1-C10-D10</f>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C15">
         <f>0.8*Phase1!B15</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>1-C11-D11</f>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B16">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C16">
         <f>0.8*Phase1!B16</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>1-C12-D12</f>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C17">
         <f>0.8*Phase1!B17</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f>1-C13-D13</f>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C18">
         <f>0.8*Phase1!B18</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f>1-C14-D14</f>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C19">
         <f>0.8*Phase1!B19</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <f>1-C15-D15</f>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C20">
         <f>0.8*Phase1!B20</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f>1-C16-D16</f>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <f>0.8*Phase1!B21</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <f>1-C17-D17</f>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B18">
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C22">
         <f>0.8*Phase1!B22</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f>1-C18-D18</f>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="C23">
         <f>0.8*Phase1!B23</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f>1-C19-D19</f>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C24">
         <f>0.8*Phase1!B24</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f>1-C20-D20</f>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C21">
+      <c r="C25">
         <f>0.8*Phase1!B25</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f>1-C21-D21</f>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C26">
         <f>0.8*Phase1!B26</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D22">
+      <c r="D26">
         <v>0.01</v>
       </c>
-      <c r="E22">
-        <f>1-C22-D22</f>
+      <c r="E26">
+        <f t="shared" si="2"/>
         <v>0.98760000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C27">
         <f>0.8*Phase1!B27</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D23">
+      <c r="D27">
         <v>0.01</v>
       </c>
-      <c r="E23">
-        <f>1-C23-D23</f>
+      <c r="E27">
+        <f t="shared" si="2"/>
         <v>0.98760000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B24">
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C28">
         <f>0.8*Phase1!B28</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E24">
-        <f>1-C24-D24</f>
+      <c r="E28">
+        <f t="shared" si="2"/>
         <v>0.98260000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B25">
+      <c r="B29">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C29">
         <f>0.8*Phase1!B29</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E25">
-        <f>1-C25-D25</f>
+      <c r="E29">
+        <f t="shared" si="2"/>
         <v>0.98260000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B26">
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <f>0.8*Phase1!B30</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>0.02</v>
       </c>
-      <c r="E26">
-        <f>1-C26-D26</f>
+      <c r="E30">
+        <f t="shared" si="2"/>
         <v>0.97760000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B27">
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="C27">
+      <c r="C31">
         <f>0.8*Phase1!B31</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D27">
+      <c r="D31">
         <v>0.02</v>
       </c>
-      <c r="E27">
-        <f>1-C27-D27</f>
+      <c r="E31">
+        <f t="shared" si="2"/>
         <v>0.97760000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B28">
+      <c r="B32">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C32">
         <f>0.8*Phase1!B32</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D28">
+      <c r="D32">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E28">
-        <f>1-C28-D28</f>
+      <c r="E32">
+        <f t="shared" si="2"/>
         <v>0.97260000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B29">
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C29">
+      <c r="C33">
         <f>0.8*Phase1!B33</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D29">
+      <c r="D33">
         <v>0.03</v>
       </c>
-      <c r="E29">
-        <f>1-C29-D29</f>
+      <c r="E33">
+        <f t="shared" si="2"/>
         <v>0.96760000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B30">
+      <c r="B34">
         <v>1</v>
       </c>
-      <c r="C30">
+      <c r="C34">
         <f>0.8*Phase1!B34</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D30">
+      <c r="D34">
         <v>0.09</v>
       </c>
-      <c r="E30">
-        <f>1-C30-D30</f>
+      <c r="E34">
+        <f t="shared" si="2"/>
         <v>0.90760000000000007</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B31">
+      <c r="B35">
         <v>1</v>
       </c>
-      <c r="C31">
+      <c r="C35">
         <f>0.8*Phase1!B35</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D31">
+      <c r="D35">
         <v>0.09</v>
       </c>
-      <c r="E31">
-        <f>1-C31-D31</f>
+      <c r="E35">
+        <f t="shared" si="2"/>
         <v>0.90760000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B32">
+      <c r="B36">
         <v>1</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <f>0.8*Phase1!B36</f>
         <v>2.4000000000000002E-3</v>
       </c>
-      <c r="D32">
+      <c r="D36">
         <v>0.09</v>
       </c>
-      <c r="E32">
-        <f>1-C32-D32</f>
+      <c r="E36">
+        <f t="shared" si="2"/>
         <v>0.90760000000000007</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B33">
+      <c r="B37">
         <v>1</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <f>0.8*Phase1!B37</f>
         <v>1.6800000000000002E-4</v>
       </c>
-      <c r="D33">
+      <c r="D37">
         <v>0.3</v>
       </c>
-      <c r="E33">
-        <f>1-C33-D33</f>
+      <c r="E37">
+        <f t="shared" si="2"/>
         <v>0.69983200000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>36</v>
       </c>
-      <c r="B34">
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C34">
+      <c r="C38">
         <f>0.8*Phase1!B38</f>
         <v>2.1600000000000002E-4</v>
       </c>
-      <c r="D34">
+      <c r="D38">
         <v>0.35</v>
       </c>
-      <c r="E34">
-        <f>1-C34-D34</f>
+      <c r="E38">
+        <f t="shared" si="2"/>
         <v>0.64978400000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>37</v>
       </c>
-      <c r="B35">
+      <c r="B39">
         <v>1</v>
       </c>
-      <c r="C35">
+      <c r="C39">
         <f>0.8*Phase1!B39</f>
         <v>2.8000000000000003E-4</v>
       </c>
-      <c r="D35">
+      <c r="D39">
         <v>0.7</v>
       </c>
-      <c r="E35">
-        <f>1-C35-D35</f>
+      <c r="E39">
+        <f t="shared" si="2"/>
         <v>0.2997200000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>38</v>
       </c>
-      <c r="B36">
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="C36">
+      <c r="C40">
         <f>0.8*Phase1!B40</f>
         <v>3.3600000000000004E-4</v>
       </c>
-      <c r="D36">
+      <c r="D40">
         <v>0.7</v>
       </c>
-      <c r="E36">
-        <f>1-C36-D36</f>
+      <c r="E40">
+        <f t="shared" si="2"/>
         <v>0.29966400000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>39</v>
       </c>
-      <c r="B37">
+      <c r="B41">
         <v>1</v>
       </c>
-      <c r="C37">
+      <c r="C41">
         <f>0.8*Phase1!B41</f>
         <v>4.8799999999999999E-4</v>
       </c>
-      <c r="D37">
+      <c r="D41">
         <v>0.7</v>
       </c>
-      <c r="E37">
-        <f>1-C37-D37</f>
+      <c r="E41">
+        <f t="shared" si="2"/>
         <v>0.299512</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B38">
+      <c r="B42">
         <v>1</v>
       </c>
-      <c r="C38">
+      <c r="C42">
         <f>0.8*Phase1!B42</f>
         <v>8.6400000000000008E-4</v>
       </c>
-      <c r="D38">
-        <f>1-C38</f>
+      <c r="D42">
+        <f>1-C42</f>
         <v>0.99913600000000002</v>
       </c>
-      <c r="E38">
+      <c r="E42">
         <v>0</v>
       </c>
     </row>
@@ -3476,20 +3684,20 @@
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K1" t="s">
@@ -3497,10 +3705,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3533,8 +3741,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4348,6 +4556,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -4572,16 +4789,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4598,12 +4814,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Wrote code to implement Phase 3. Still needs to be reviewed for potential edge cases and bugs.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB50349B-7940-B24B-B465-024B1710078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E469F0-A911-3548-A860-24044D5A6DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -148,7 +148,7 @@
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,7 +156,7 @@
     https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -369,6 +369,15 @@
   </si>
   <si>
     <t>p_index</t>
+  </si>
+  <si>
+    <t>treat_effect_OR</t>
+  </si>
+  <si>
+    <t>treat_effect_ln_OR</t>
+  </si>
+  <si>
+    <t>ln_odds_preeclampsia</t>
   </si>
 </sst>
 </file>
@@ -795,10 +804,10 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2023-10-27T16:29:57.16" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
+  <threadedComment ref="B1" dT="2023-10-27T16:29:57.16" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
     <text>https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2023-10-27T12:57:42.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+  <threadedComment ref="F1" dT="2023-10-27T12:57:42.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/</text>
   </threadedComment>
 </ThreadedComments>
@@ -1634,7 +1643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -2447,321 +2456,458 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEC42C-213B-4245-8F9C-C0F65FBC0D09}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <v>4.0000000000000002E-4</v>
+        <f>LN(B2/(1-B2))</f>
+        <v>-7.8236459308349522</v>
       </c>
       <c r="D2">
+        <v>0.7</v>
+      </c>
+      <c r="E2">
+        <f>LN(D2)</f>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E17" si="0">1-D2</f>
+      <c r="G2">
+        <f t="shared" ref="G2:G17" si="0">1-F2</f>
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3">
-        <v>5.0000000000000001E-4</v>
+        <f t="shared" ref="C3:C17" si="1">LN(B3/(1-B3))</f>
+        <v>-7.6004023345003997</v>
       </c>
       <c r="D3">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3:E17" si="2">LN(D3)</f>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G3">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>27</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="C4">
-        <v>5.9999999999999995E-4</v>
+        <f t="shared" si="1"/>
+        <v>-7.417980722676095</v>
       </c>
       <c r="D4">
+        <v>0.7</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>0.996</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>28</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="C5">
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="1"/>
+        <v>-7.2637299778064763</v>
       </c>
       <c r="D5">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E5">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>29</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C6">
-        <v>8.0000000000000004E-4</v>
+        <f t="shared" si="1"/>
+        <v>-7.1300985101255776</v>
       </c>
       <c r="D6">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E6">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>30</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="C7">
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="1"/>
+        <v>-7.0122153893967996</v>
       </c>
       <c r="D7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E7">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>31</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C8">
-        <v>1E-3</v>
+        <f t="shared" si="1"/>
+        <v>-6.9067547786485539</v>
       </c>
       <c r="D8">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>32</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1.8E-3</v>
       </c>
       <c r="C9">
-        <v>1.8E-3</v>
+        <f t="shared" si="1"/>
+        <v>-6.3181669921333894</v>
       </c>
       <c r="D9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E9">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>33</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="C10">
-        <v>2E-3</v>
+        <f t="shared" si="1"/>
+        <v>-6.2126060957515188</v>
       </c>
       <c r="D10">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E10">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>34</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C11">
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>-5.5174528964647074</v>
       </c>
       <c r="D11">
-        <v>3.0000000000000001E-3</v>
+        <v>0.7</v>
       </c>
       <c r="E11">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C12">
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>-5.2933048247244923</v>
       </c>
       <c r="D12">
+        <v>0.7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F12">
         <v>1E-3</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>36</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C13">
-        <v>7.0000000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>-4.9548205149898594</v>
       </c>
       <c r="D13">
+        <v>0.7</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F13">
         <v>1E-3</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>37</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C14">
-        <v>8.0000000000000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>-4.8202815656050371</v>
       </c>
       <c r="D14">
+        <v>0.7</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F14">
         <v>1E-3</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>38</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="C15">
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="1"/>
+        <v>-7.0122153893967996</v>
       </c>
       <c r="D15">
+        <v>0.7</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F15">
         <v>1E-3</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C16">
-        <v>1.0999999999999999E-2</v>
+        <f t="shared" si="1"/>
+        <v>-4.4987990588243418</v>
       </c>
       <c r="D16">
+        <v>0.7</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F16">
         <v>2E-3</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <f t="shared" si="0"/>
         <v>0.998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="C17">
-        <v>1.4E-2</v>
+        <f t="shared" si="1"/>
+        <v>-4.2545990249873764</v>
       </c>
       <c r="D17">
+        <v>0.7</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="F17">
         <v>1E-3</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
@@ -2777,7 +2923,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
De-bugging. Some functions returning unexpected NAs. Needs continued work.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E469F0-A911-3548-A860-24044D5A6DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC75FFE-17A1-5E4E-9624-20293B320BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="3" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -161,7 +161,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/</t>
+    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/
+Reply:
+    Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</t>
       </text>
     </comment>
   </commentList>
@@ -279,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -379,6 +381,9 @@
   <si>
     <t>ln_odds_preeclampsia</t>
   </si>
+  <si>
+    <t>trt_value</t>
+  </si>
 </sst>
 </file>
 
@@ -414,12 +419,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -434,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +455,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,6 +822,9 @@
   <threadedComment ref="F1" dT="2023-10-27T12:57:42.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/</text>
   </threadedComment>
+  <threadedComment ref="F1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+    <text>Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2458,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEC42C-213B-4245-8F9C-C0F65FBC0D09}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2489,7 +2504,7 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
@@ -2922,15 +2937,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Conducted basic descriptive analyses. Datasets behaving as expected.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC75FFE-17A1-5E4E-9624-20293B320BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C6688F-2A82-2D4D-B8BF-8B6032C217E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="3" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,6 +45,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}</author>
+    <author>tc={185333BF-83E7-AF45-9DD5-668399EC57D8}</author>
+    <author>tc={5A01CF90-F8E3-6640-BC32-993409305B38}</author>
     <author>tc={50F77D56-3B06-6E4B-8155-7833EAB9408D}</author>
     <author>tc={73131F6C-4FDD-8242-81D0-C94D07ECA3E3}</author>
     <author>tc={D6D95E37-6D2A-4548-AFD1-5EE5DA643221}</author>
@@ -57,7 +60,23 @@
     https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="1" shapeId="0" xr:uid="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{185333BF-83E7-AF45-9DD5-668399EC57D8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.3. Same with gw 1</t>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="2" shapeId="0" xr:uid="{5A01CF90-F8E3-6640-BC32-993409305B38}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lowered this slightly from 0.2 to 0.15 to improve sample size.</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="3" shapeId="0" xr:uid="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -65,7 +84,7 @@
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
       </text>
     </comment>
-    <comment ref="C26" authorId="2" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
+    <comment ref="C26" authorId="4" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -73,7 +92,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="3" shapeId="0" xr:uid="{D6D95E37-6D2A-4548-AFD1-5EE5DA643221}">
+    <comment ref="B37" authorId="5" shapeId="0" xr:uid="{D6D95E37-6D2A-4548-AFD1-5EE5DA643221}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -145,6 +164,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={64BAD85A-477D-3B47-ACFB-F7563888EB93}</author>
+    <author>tc={4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}</author>
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
   </authors>
   <commentList>
@@ -156,7 +176,17 @@
     https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Increased the risk of preeclampsia for the simulation
+Reply:
+    Ideally, want to be at 10-25% of untreated with preeclampsia: High blood pressure: A risk factor for preeclampsiaMarch of Dimeshttps://www.marchofdimes.org › find-support › blog › h...</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="2" shapeId="0" xr:uid="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -171,6 +201,24 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BF5B5001-B1EA-1F47-AB8D-821418E22C5D}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BF5B5001-B1EA-1F47-AB8D-821418E22C5D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maybe treatment shouldn’t have an effect on SGA?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E6E88FEF-63DE-2F45-80DF-11FAF199CED4}</author>
@@ -243,7 +291,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={7F21C0C9-3748-7449-8B61-7AC75D94AA52}</author>
@@ -281,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -384,12 +432,15 @@
   <si>
     <t>trt_value</t>
   </si>
+  <si>
+    <t>p_preeclampsia_original</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,6 +468,12 @@
       <color rgb="FF212121"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -453,9 +510,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,6 +836,12 @@
   <threadedComment ref="B1" dT="2023-10-20T20:28:15.91" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}">
     <text>https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</text>
   </threadedComment>
+  <threadedComment ref="B2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{185333BF-83E7-AF45-9DD5-668399EC57D8}">
+    <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.3. Same with gw 1</text>
+  </threadedComment>
+  <threadedComment ref="B4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{5A01CF90-F8E3-6640-BC32-993409305B38}">
+    <text>Lowered this slightly from 0.2 to 0.15 to improve sample size.</text>
+  </threadedComment>
   <threadedComment ref="B21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
@@ -819,16 +882,36 @@
   <threadedComment ref="B1" dT="2023-10-27T16:29:57.16" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
     <text>https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</text>
   </threadedComment>
-  <threadedComment ref="F1" dT="2023-10-27T12:57:42.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+  <threadedComment ref="C1" dT="2023-11-27T01:54:37.91" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}">
+    <text>Increased the risk of preeclampsia for the simulation</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2023-11-27T01:59:11.30" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{87DE33D1-1F43-EB47-9370-EDEB086C1788}" parentId="{4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}">
+    <text>Ideally, want to be at 10-25% of untreated with preeclampsia: High blood pressure: A risk factor for preeclampsiaMarch of Dimeshttps://www.marchofdimes.org › find-support › blog › h...</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>404583031</xltc2:checksum>
+        <xltc2:hyperlink startIndex="62" length="122" url="https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;cad=rja&amp;uact=8&amp;ved=2ahUKEwj9ucGciuOCAxU1lGoFHVFcDqoQFnoECA8QAw&amp;url=https%3A%2F%2Fwww.marchofdimes.org%2Ffind-support%2Fblog%2Fhigh-blood-pressure-risk-factor-preeclampsia-0%23%3A~%3Atext%3DAccording%2520to%2520the%2520American%2520College%2Caspirin%2520to%2520help%2520prevent%2520it.&amp;usg=AOvVaw2WnPBfo15qNAd5MeG9CtOf&amp;opi=89978449"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2023-10-27T12:57:42.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/</text>
   </threadedComment>
-  <threadedComment ref="F1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+  <threadedComment ref="G1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-11-27T02:03:33.50" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BF5B5001-B1EA-1F47-AB8D-821418E22C5D}">
+    <text>Maybe treatment shouldn’t have an effect on SGA?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="B1" dT="2023-10-20T20:28:15.91" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6E88FEF-63DE-2F45-80DF-11FAF199CED4}">
     <text>https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</text>
@@ -861,7 +944,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2023-10-27T12:40:23.55" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{7F21C0C9-3748-7449-8B61-7AC75D94AA52}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/#:~:text=However%2C%20relative%20risk%20of%20stillbirth,CI%3D46%20to%20142).</text>
@@ -881,7 +964,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,14 +997,14 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <f>1-C2-B2</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -932,14 +1015,14 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D6" si="0">1-C3-B3</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -950,14 +1033,14 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -968,14 +1051,14 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1659,7 +1742,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1696,14 +1779,14 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <f>1-D2-C2</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1714,14 +1797,14 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="0">1-D3-C3</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1732,14 +1815,14 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1750,14 +1833,14 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2471,47 +2554,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEC42C-213B-4245-8F9C-C0F65FBC0D09}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>25</v>
       </c>
@@ -2519,25 +2606,29 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <f>LN(B2/(1-B2))</f>
-        <v>-7.8236459308349522</v>
+        <f>15*B2</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D2">
-        <v>0.7</v>
+        <f>LN(C2/(1-C2))</f>
+        <v>-5.1099777374285189</v>
       </c>
       <c r="E2">
-        <f>LN(D2)</f>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F2">
+        <f>LN(E2)</f>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G17" si="0">1-F2</f>
+      <c r="H2">
+        <f t="shared" ref="H2:H17" si="0">1-G2</f>
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>26</v>
       </c>
@@ -2545,25 +2636,29 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" si="1">LN(B3/(1-B3))</f>
-        <v>-7.6004023345003997</v>
+        <f t="shared" ref="C3:C17" si="1">15*B3</f>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="D3">
-        <v>0.7</v>
+        <f t="shared" ref="D3:D17" si="2">LN(C3/(1-C3))</f>
+        <v>-4.8853239920190807</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E17" si="2">LN(D3)</f>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F3">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" ref="F3:F17" si="3">LN(E3)</f>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H3">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>27</v>
       </c>
@@ -2572,24 +2667,28 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>-7.417980722676095</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D4">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.7014899569937691</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F4">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>0.996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>28</v>
       </c>
@@ -2598,24 +2697,28 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>-7.2637299778064763</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="D5">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.5458245078791428</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F5">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>29</v>
       </c>
@@ -2624,24 +2727,28 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>-7.1300985101255776</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D6">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.4107760479598674</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F6">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>30</v>
       </c>
@@ -2650,24 +2757,28 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>-7.0122153893967996</v>
+        <v>1.35E-2</v>
       </c>
       <c r="D7">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.2914736400182862</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F7">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>31</v>
       </c>
@@ -2676,24 +2787,28 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-6.9067547786485539</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.1845914400698785</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F8">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>32</v>
       </c>
@@ -2702,24 +2817,28 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-6.3181669921333894</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D9">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-3.5845472161816758</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F9">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>33</v>
       </c>
@@ -2728,24 +2847,28 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-6.2126060957515188</v>
+        <v>0.03</v>
       </c>
       <c r="D10">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-3.4760986898352733</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F10">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>34</v>
       </c>
@@ -2754,24 +2877,28 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>-5.5174528964647074</v>
+        <v>0.06</v>
       </c>
       <c r="D11">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-2.7515353130419489</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F11">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>35</v>
       </c>
@@ -2780,24 +2907,28 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>-5.2933048247244923</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D12">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-2.5123056239761148</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F12">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G12">
         <v>1E-3</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>36</v>
       </c>
@@ -2806,24 +2937,28 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>-4.9548205149898594</v>
+        <v>0.105</v>
       </c>
       <c r="D13">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-2.1428633681173319</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F13">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G13">
         <v>1E-3</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>37</v>
       </c>
@@ -2832,24 +2967,28 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>-4.8202815656050371</v>
+        <v>0.12</v>
       </c>
       <c r="D14">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-1.9924301646902063</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F14">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G14">
         <v>1E-3</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>38</v>
       </c>
@@ -2858,24 +2997,28 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>-7.0122153893967996</v>
+        <v>1.35E-2</v>
       </c>
       <c r="D15">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-4.2914736400182862</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F15">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G15">
         <v>1E-3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39</v>
       </c>
@@ -2884,24 +3027,28 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>-4.4987990588243418</v>
+        <v>0.16499999999999998</v>
       </c>
       <c r="D16">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-1.621486250950275</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F16">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G16">
         <v>2E-3</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>0.998</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -2910,19 +3057,23 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>-4.2545990249873764</v>
+        <v>0.21</v>
       </c>
       <c r="D17">
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>-1.3249254147435987</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>-0.35667494393873245</v>
+        <v>0.6</v>
       </c>
       <c r="F17">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="G17">
         <v>1E-3</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>0.999</v>
       </c>
@@ -2934,12 +3085,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2948,7 +3097,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
@@ -3007,6 +3156,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3849,19 +3999,19 @@
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
@@ -3870,10 +4020,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3906,8 +4056,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Added some additional analyses for discussion.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C6688F-2A82-2D4D-B8BF-8B6032C217E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B199F7B3-93C9-2B46-879F-8FCC32965C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="540" windowWidth="28040" windowHeight="16180" activeTab="3" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -211,7 +211,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Maybe treatment shouldn’t have an effect on SGA?</t>
+    Maybe treatment shouldn’t have an effect on SGA?
+Reply:
+    I think the counter-argument for a treatment effect was that the results weren’t really interesting to discuss without a treatment effect.</t>
       </text>
     </comment>
   </commentList>
@@ -908,6 +910,9 @@
   <threadedComment ref="A1" dT="2023-11-27T02:03:33.50" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BF5B5001-B1EA-1F47-AB8D-821418E22C5D}">
     <text>Maybe treatment shouldn’t have an effect on SGA?</text>
   </threadedComment>
+  <threadedComment ref="A1" dT="2023-11-27T02:28:42.57" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{21A0BB0A-4B0F-E74C-8D6A-B40C2502836C}" parentId="{BF5B5001-B1EA-1F47-AB8D-821418E22C5D}">
+    <text>I think the counter-argument for a treatment effect was that the results weren’t really interesting to discuss without a treatment effect.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1741,7 +1746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3088,7 +3093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Added a sheet for censoring throughout pregnancy.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE86A545-FC15-D644-A060-29316B35560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE4A46B-047E-5D4F-BDCD-8AC1678ADCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
     <sheet name="Phase2" sheetId="2" r:id="rId2"/>
     <sheet name="Phase3" sheetId="3" r:id="rId3"/>
     <sheet name="Phase4" sheetId="5" r:id="rId4"/>
-    <sheet name="OLD" sheetId="1" r:id="rId5"/>
-    <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId6"/>
+    <sheet name="Phase 5" sheetId="7" r:id="rId5"/>
+    <sheet name="OLD" sheetId="1" r:id="rId6"/>
+    <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -330,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -435,6 +436,9 @@
   </si>
   <si>
     <t>p_preeclampsia_original</t>
+  </si>
+  <si>
+    <t>p_censoring</t>
   </si>
 </sst>
 </file>
@@ -961,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A42"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3116,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -3191,6 +3195,361 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C0E0C-D6E1-F442-8735-4FA62BD9AC1D}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFC6947-DBBF-D243-8019-94691EC417BF}">
   <dimension ref="A1:F38"/>
   <sheetViews>
@@ -4009,7 +4368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0657A824-9110-B347-821D-B64D54D407AE}">
   <dimension ref="A1:L23"/>
   <sheetViews>
@@ -4901,6 +5260,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5125,16 +5493,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5151,12 +5518,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Created R code to generate censoring events
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE4A46B-047E-5D4F-BDCD-8AC1678ADCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416E4200-6C20-0746-BE97-771A477920E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Phase2" sheetId="2" r:id="rId2"/>
     <sheet name="Phase3" sheetId="3" r:id="rId3"/>
     <sheet name="Phase4" sheetId="5" r:id="rId4"/>
-    <sheet name="Phase 5" sheetId="7" r:id="rId5"/>
+    <sheet name="Phase5" sheetId="7" r:id="rId5"/>
     <sheet name="OLD" sheetId="1" r:id="rId6"/>
     <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -3198,8 +3198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C0E0C-D6E1-F442-8735-4FA62BD9AC1D}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3541,7 +3541,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created functions for AJ estimator of risks and RRs
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416E4200-6C20-0746-BE97-771A477920E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06821346-AB23-AC46-8766-23305A22878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -3199,7 +3199,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3269,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3277,7 +3277,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3285,7 +3285,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3293,7 +3293,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3309,7 +3309,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3317,7 +3317,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3325,7 +3325,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3333,7 +3333,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3341,7 +3341,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3349,7 +3349,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3357,7 +3357,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3365,7 +3365,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3373,7 +3373,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3381,7 +3381,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3389,7 +3389,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3397,7 +3397,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3405,7 +3405,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3413,7 +3413,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3421,7 +3421,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3429,7 +3429,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -3437,7 +3437,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3445,7 +3445,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3453,7 +3453,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3461,7 +3461,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3469,7 +3469,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3477,7 +3477,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3485,7 +3485,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -3493,7 +3493,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -3501,7 +3501,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -3509,7 +3509,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -3517,7 +3517,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -3525,7 +3525,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3533,7 +3533,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Considering different analyses. De-bugged a few analysis functions.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06821346-AB23-AC46-8766-23305A22878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418AFCEA-B5A5-7B4C-B24D-7D6A21F9E623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -65,7 +65,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.3. Same with gw 1</t>
+    Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</t>
       </text>
     </comment>
     <comment ref="B4" authorId="2" shapeId="0" xr:uid="{5A01CF90-F8E3-6640-BC32-993409305B38}">
@@ -73,7 +73,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Lowered this slightly from 0.2 to 0.15 to improve sample size.</t>
+    Lowered this slightly from 0.2 to 0.1 to improve sample size.</t>
       </text>
     </comment>
     <comment ref="B21" authorId="3" shapeId="0" xr:uid="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
@@ -109,6 +109,8 @@
   <authors>
     <author>tc={2761945B-CCCA-C740-B794-13037E1324C6}</author>
     <author>tc={642DC8BF-9352-A841-B7D5-D2353D7406FD}</author>
+    <author>tc={6E365861-8AD7-9741-8A7F-D39E04493C98}</author>
+    <author>tc={34791295-B5FE-8945-B66F-FD8231C95036}</author>
     <author>tc={4C6D7E70-155D-F143-8348-12998FB8F68A}</author>
     <author>tc={0750D8B8-3F43-0249-A235-DC6D645DAACD}</author>
     <author>tc={2685FFE7-F524-DD45-9B6C-36B63629A0C0}</author>
@@ -132,7 +134,23 @@
     Values for gw 0-4 are the same because people wouldn’t actually be treated at this point, even if they entered the trial. This will be dealt with on the coding side.</t>
       </text>
     </comment>
-    <comment ref="C21" authorId="2" shapeId="0" xr:uid="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{6E365861-8AD7-9741-8A7F-D39E04493C98}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="3" shapeId="0" xr:uid="{34791295-B5FE-8945-B66F-FD8231C95036}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lowered this slightly from 0.2 to 0.1 to improve sample size.</t>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="4" shapeId="0" xr:uid="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,15 +158,17 @@
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
       </text>
     </comment>
-    <comment ref="D26" authorId="3" shapeId="0" xr:uid="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
+    <comment ref="D26" authorId="5" shapeId="0" xr:uid="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
+    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.
+Reply:
+    Going to have it decrease the risk of preterm birth</t>
       </text>
     </comment>
-    <comment ref="C37" authorId="4" shapeId="0" xr:uid="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
+    <comment ref="C37" authorId="6" shapeId="0" xr:uid="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -445,7 +465,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,6 +493,12 @@
       <color rgb="FF212121"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -836,10 +862,10 @@
     <text>https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</text>
   </threadedComment>
   <threadedComment ref="B2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{185333BF-83E7-AF45-9DD5-668399EC57D8}">
-    <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.3. Same with gw 1</text>
+    <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
   </threadedComment>
   <threadedComment ref="B4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{5A01CF90-F8E3-6640-BC32-993409305B38}">
-    <text>Lowered this slightly from 0.2 to 0.15 to improve sample size.</text>
+    <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
   </threadedComment>
   <threadedComment ref="B21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
@@ -864,11 +890,20 @@
   <threadedComment ref="A2" dT="2023-11-25T18:21:45.43" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{642DC8BF-9352-A841-B7D5-D2353D7406FD}">
     <text>Values for gw 0-4 are the same because people wouldn’t actually be treated at this point, even if they entered the trial. This will be dealt with on the coding side.</text>
   </threadedComment>
+  <threadedComment ref="C2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{6E365861-8AD7-9741-8A7F-D39E04493C98}">
+    <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
+  </threadedComment>
+  <threadedComment ref="C4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{34791295-B5FE-8945-B66F-FD8231C95036}">
+    <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
+  </threadedComment>
   <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{4C6D7E70-155D-F143-8348-12998FB8F68A}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
   <threadedComment ref="D26" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</text>
+  </threadedComment>
+  <threadedComment ref="D26" dT="2023-12-15T03:39:36.56" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D51B01E8-6637-E44B-A544-4E4553ED1B10}" parentId="{0750D8B8-3F43-0249-A235-DC6D645DAACD}">
+    <text>Going to have it decrease the risk of preterm birth</text>
   </threadedComment>
   <threadedComment ref="C37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2685FFE7-F524-DD45-9B6C-36B63629A0C0}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</text>
@@ -963,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,14 +1034,14 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <f>1-C2-B2</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1017,14 +1052,14 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D6" si="0">1-C3-B3</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1035,14 +1070,14 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1053,14 +1088,14 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1264,7 +1299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1282,7 +1317,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1300,7 +1335,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1318,7 +1353,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1336,7 +1371,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1354,7 +1389,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1372,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1390,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1408,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1425,8 +1460,12 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <f>0.8*C26</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1444,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1462,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1480,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1498,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1516,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1534,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1741,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1781,14 +1820,14 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <f>1-D2-C2</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1799,14 +1838,14 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="0">1-D3-C3</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1817,14 +1856,14 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1835,14 +1874,14 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2054,7 +2093,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2073,7 +2112,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2092,7 +2131,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2111,7 +2150,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2130,7 +2169,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2149,7 +2188,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2167,8 +2206,12 @@
         <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f>1/0.8</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2187,7 +2230,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2206,7 +2249,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2225,7 +2268,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2237,14 +2280,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D26">
-        <v>0.01</v>
+        <f>0.7*Phase1!C26</f>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>0.98760000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99060000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2256,14 +2300,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D27">
-        <v>0.01</v>
+        <f>0.7*Phase1!C27</f>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>0.98760000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99060000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2275,14 +2320,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D28">
-        <v>1.4999999999999999E-2</v>
+        <f>0.7*Phase1!C28</f>
+        <v>1.0499999999999999E-2</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>0.98260000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98710000000000009</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2294,14 +2340,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D29">
-        <v>1.4999999999999999E-2</v>
+        <f>0.7*Phase1!C29</f>
+        <v>1.0499999999999999E-2</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>0.98260000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98710000000000009</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2313,14 +2360,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D30">
-        <v>0.02</v>
+        <f>0.7*Phase1!C30</f>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>0.97760000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98360000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2332,14 +2380,15 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D31">
-        <v>0.02</v>
+        <f>0.7*Phase1!C31</f>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>0.97760000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98360000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2351,11 +2400,12 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D32">
-        <v>2.5000000000000001E-2</v>
+        <f>0.7*Phase1!C32</f>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>0.97260000000000002</v>
+        <v>0.98010000000000008</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2370,11 +2420,12 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D33">
-        <v>0.03</v>
+        <f>0.7*Phase1!C33</f>
+        <v>2.0999999999999998E-2</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>0.96760000000000002</v>
+        <v>0.97660000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2389,11 +2440,12 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D34">
-        <v>0.09</v>
+        <f>0.7*Phase1!C34</f>
+        <v>6.3E-2</v>
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
-        <v>0.90760000000000007</v>
+        <v>0.9346000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2408,11 +2460,12 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D35">
-        <v>0.09</v>
+        <f>0.7*Phase1!C35</f>
+        <v>6.3E-2</v>
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
-        <v>0.90760000000000007</v>
+        <v>0.9346000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2427,11 +2480,12 @@
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="D36">
-        <v>0.09</v>
+        <f>0.7*Phase1!C36</f>
+        <v>6.3E-2</v>
       </c>
       <c r="E36">
         <f t="shared" si="2"/>
-        <v>0.90760000000000007</v>
+        <v>0.9346000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2446,11 +2500,12 @@
         <v>1.6800000000000002E-4</v>
       </c>
       <c r="D37">
-        <v>0.3</v>
+        <f>0.7*Phase1!C37</f>
+        <v>0.21</v>
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
-        <v>0.69983200000000001</v>
+        <v>0.78983200000000009</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2465,11 +2520,12 @@
         <v>2.1600000000000002E-4</v>
       </c>
       <c r="D38">
-        <v>0.35</v>
+        <f>0.7*Phase1!C38</f>
+        <v>0.24499999999999997</v>
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
-        <v>0.64978400000000003</v>
+        <v>0.75478400000000001</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2483,7 +2539,8 @@
         <f>0.8*Phase1!B39</f>
         <v>2.8000000000000003E-4</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="5">
+        <f>Phase1!C39</f>
         <v>0.7</v>
       </c>
       <c r="E39">
@@ -2502,7 +2559,8 @@
         <f>0.8*Phase1!B40</f>
         <v>3.3600000000000004E-4</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="5">
+        <f>Phase1!C40</f>
         <v>0.7</v>
       </c>
       <c r="E40">
@@ -2521,7 +2579,8 @@
         <f>0.8*Phase1!B41</f>
         <v>4.8799999999999999E-4</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="5">
+        <f>Phase1!C41</f>
         <v>0.7</v>
       </c>
       <c r="E41">
@@ -3121,7 +3180,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3149,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3161,7 +3220,7 @@
       </c>
       <c r="C3">
         <f>1.25*C2</f>
-        <v>0.125</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3172,8 +3231,8 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f>0.9*C2</f>
-        <v>9.0000000000000011E-2</v>
+        <f>0.8*C2</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3184,8 +3243,8 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>0.9*1.25*C2</f>
-        <v>0.1125</v>
+        <f>0.8*C3</f>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -3198,7 +3257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C0E0C-D6E1-F442-8735-4FA62BD9AC1D}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -5260,15 +5319,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5493,15 +5543,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5518,4 +5569,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Some de-bugging of analysis functions. Not sure if everything performing as expected. Ran through a few possible scenarios.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418AFCEA-B5A5-7B4C-B24D-7D6A21F9E623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78523F-5C68-FF4D-91B1-4654C414C82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -45,11 +45,16 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}</author>
-    <author>tc={185333BF-83E7-AF45-9DD5-668399EC57D8}</author>
-    <author>tc={5A01CF90-F8E3-6640-BC32-993409305B38}</author>
-    <author>tc={50F77D56-3B06-6E4B-8155-7833EAB9408D}</author>
+    <author>tc={9A5BA4F2-D71D-6E40-92FE-646A717AC649}</author>
+    <author>tc={AA203F26-57EB-FD4D-96A8-1E3EC58078F0}</author>
+    <author>tc={136807CB-0C11-AF4B-B455-BA7E6BADFC55}</author>
+    <author>tc={A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}</author>
+    <author>tc={E0F99EF9-03C3-8340-B100-DF68AE4D4DF8}</author>
+    <author>tc={BA1965E4-CB1E-A446-858D-2C189AC85BC3}</author>
+    <author>tc={B884D584-EC30-294D-8EAD-B0E58A3378E6}</author>
+    <author>tc={AAEBD684-F7D6-6E4D-896A-3757334CE7FF}</author>
     <author>tc={73131F6C-4FDD-8242-81D0-C94D07ECA3E3}</author>
-    <author>tc={D6D95E37-6D2A-4548-AFD1-5EE5DA643221}</author>
+    <author>tc={F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}">
@@ -60,7 +65,7 @@
     https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</t>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{185333BF-83E7-AF45-9DD5-668399EC57D8}">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +73,7 @@
     Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</t>
       </text>
     </comment>
-    <comment ref="B4" authorId="2" shapeId="0" xr:uid="{5A01CF90-F8E3-6640-BC32-993409305B38}">
+    <comment ref="B4" authorId="2" shapeId="0" xr:uid="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +81,31 @@
     Lowered this slightly from 0.2 to 0.1 to improve sample size.</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="3" shapeId="0" xr:uid="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
+    <comment ref="E4" authorId="3" shapeId="0" xr:uid="{136807CB-0C11-AF4B-B455-BA7E6BADFC55}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0 because got confused on gw from conception and from LMP</t>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="4" shapeId="0" xr:uid="{A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0 because got confused on gw from conception and from LMP</t>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="5" shapeId="0" xr:uid="{E0F99EF9-03C3-8340-B100-DF68AE4D4DF8}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.5. However, increased it to 1 because this is 20 gw from LMP. </t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="6" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,7 +113,23 @@
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
       </text>
     </comment>
-    <comment ref="C26" authorId="4" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
+    <comment ref="E21" authorId="7" shapeId="0" xr:uid="{B884D584-EC30-294D-8EAD-B0E58A3378E6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.5. See above</t>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="8" shapeId="0" xr:uid="{AAEBD684-F7D6-6E4D-896A-3757334CE7FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 1. See above comment.</t>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="9" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,7 +137,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="5" shapeId="0" xr:uid="{D6D95E37-6D2A-4548-AFD1-5EE5DA643221}">
+    <comment ref="B37" authorId="10" shapeId="0" xr:uid="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -861,19 +906,34 @@
   <threadedComment ref="B1" dT="2023-10-20T20:28:15.91" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}">
     <text>https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</text>
   </threadedComment>
-  <threadedComment ref="B2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{185333BF-83E7-AF45-9DD5-668399EC57D8}">
+  <threadedComment ref="B2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
     <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
   </threadedComment>
-  <threadedComment ref="B4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{5A01CF90-F8E3-6640-BC32-993409305B38}">
+  <threadedComment ref="B4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
     <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
   </threadedComment>
-  <threadedComment ref="B21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{50F77D56-3B06-6E4B-8155-7833EAB9408D}">
+  <threadedComment ref="E4" dT="2023-12-15T18:58:17.41" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{136807CB-0C11-AF4B-B455-BA7E6BADFC55}">
+    <text>Previously 0 because got confused on gw from conception and from LMP</text>
+  </threadedComment>
+  <threadedComment ref="E5" dT="2023-12-15T18:58:17.41" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}">
+    <text>Previously 0 because got confused on gw from conception and from LMP</text>
+  </threadedComment>
+  <threadedComment ref="E20" dT="2023-12-15T18:59:01.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E0F99EF9-03C3-8340-B100-DF68AE4D4DF8}">
+    <text xml:space="preserve">Previously 0.5. However, increased it to 1 because this is 20 gw from LMP. </text>
+  </threadedComment>
+  <threadedComment ref="B21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
+  </threadedComment>
+  <threadedComment ref="E21" dT="2023-12-15T18:59:16.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{B884D584-EC30-294D-8EAD-B0E58A3378E6}">
+    <text>Previously 0.5. See above</text>
+  </threadedComment>
+  <threadedComment ref="E22" dT="2023-12-15T18:59:30.81" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{AAEBD684-F7D6-6E4D-896A-3757334CE7FF}">
+    <text>Previously 1. See above comment.</text>
   </threadedComment>
   <threadedComment ref="C26" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</text>
   </threadedComment>
-  <threadedComment ref="B37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D6D95E37-6D2A-4548-AFD1-5EE5DA643221}">
+  <threadedComment ref="B37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</text>
   </threadedComment>
 </ThreadedComments>
@@ -998,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">1-C3-B3</f>
+        <f>1-C3-B3</f>
         <v>0.8</v>
       </c>
       <c r="E3">
@@ -1076,11 +1136,11 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>1-C4-B4</f>
         <v>0.9</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1094,11 +1154,11 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>1-C5-B5</f>
         <v>0.9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1112,11 +1172,11 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>1-C6-B6</f>
         <v>0.95</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1130,11 +1190,11 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D41" si="1">1-B7-C7</f>
+        <f>1-B7-C7</f>
         <v>0.95</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1148,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f>1-B8-C8</f>
         <v>0.97</v>
       </c>
       <c r="E8">
@@ -1166,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f>1-B9-C9</f>
         <v>0.97</v>
       </c>
       <c r="E9">
@@ -1184,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f>1-B10-C10</f>
         <v>0.97</v>
       </c>
       <c r="E10">
@@ -1202,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f>1-B11-C11</f>
         <v>0.97</v>
       </c>
       <c r="E11">
@@ -1220,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f>1-B12-C12</f>
         <v>0.97</v>
       </c>
       <c r="E12">
@@ -1238,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f>1-B13-C13</f>
         <v>0.97</v>
       </c>
       <c r="E13">
@@ -1256,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f>1-B14-C14</f>
         <v>0.99</v>
       </c>
       <c r="E14">
@@ -1274,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f>1-B15-C15</f>
         <v>0.99</v>
       </c>
       <c r="E15">
@@ -1292,14 +1352,14 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f>1-B16-C16</f>
         <v>0.99</v>
       </c>
       <c r="E16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1310,14 +1370,14 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f>1-B17-C17</f>
         <v>0.99</v>
       </c>
       <c r="E17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1328,14 +1388,14 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f>1-B18-C18</f>
         <v>0.99</v>
       </c>
       <c r="E18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1346,14 +1406,14 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f>1-B19-C19</f>
         <v>0.99</v>
       </c>
       <c r="E19">
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1364,14 +1424,14 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f>1-B20-C20</f>
         <v>0.99</v>
       </c>
       <c r="E20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1382,14 +1442,14 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f>1-B21-C21</f>
         <v>0.997</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1400,14 +1460,14 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f>1-B22-C22</f>
         <v>0.997</v>
       </c>
       <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1418,14 +1478,14 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f>1-B23-C23</f>
         <v>0.997</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1436,14 +1496,14 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f>1-B24-C24</f>
         <v>0.997</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1454,18 +1514,18 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f>1-B25-C25</f>
         <v>0.997</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="F25">
         <f>0.8*C26</f>
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1476,14 +1536,14 @@
         <v>0.01</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f>1-B26-C26</f>
         <v>0.98699999999999999</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1494,14 +1554,14 @@
         <v>0.01</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f>1-B27-C27</f>
         <v>0.98699999999999999</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1512,14 +1572,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f>1-B28-C28</f>
         <v>0.98199999999999998</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1530,14 +1590,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f>1-B29-C29</f>
         <v>0.98199999999999998</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1548,14 +1608,14 @@
         <v>0.02</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f>1-B30-C30</f>
         <v>0.97699999999999998</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1566,14 +1626,14 @@
         <v>0.02</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f>1-B31-C31</f>
         <v>0.97699999999999998</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1584,7 +1644,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f>1-B32-C32</f>
         <v>0.97199999999999998</v>
       </c>
       <c r="E32">
@@ -1602,7 +1662,7 @@
         <v>0.03</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
+        <f>1-B33-C33</f>
         <v>0.96699999999999997</v>
       </c>
       <c r="E33">
@@ -1620,7 +1680,7 @@
         <v>0.09</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
+        <f>1-B34-C34</f>
         <v>0.90700000000000003</v>
       </c>
       <c r="E34">
@@ -1638,7 +1698,7 @@
         <v>0.09</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f>1-B35-C35</f>
         <v>0.90700000000000003</v>
       </c>
       <c r="E35">
@@ -1656,7 +1716,7 @@
         <v>0.09</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f>1-B36-C36</f>
         <v>0.90700000000000003</v>
       </c>
       <c r="E36">
@@ -1675,7 +1735,7 @@
         <v>0.3</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f>1-B37-C37</f>
         <v>0.69978999999999991</v>
       </c>
       <c r="E37">
@@ -1693,7 +1753,7 @@
         <v>0.35</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f>1-B38-C38</f>
         <v>0.64973000000000003</v>
       </c>
       <c r="E38">
@@ -1711,7 +1771,7 @@
         <v>0.7</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f>1-B39-C39</f>
         <v>0.29965000000000008</v>
       </c>
       <c r="E39">
@@ -1729,7 +1789,7 @@
         <v>0.7</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f>1-B40-C40</f>
         <v>0.29958000000000007</v>
       </c>
       <c r="E40">
@@ -1747,7 +1807,7 @@
         <v>0.7</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f>1-B41-C41</f>
         <v>0.29939000000000004</v>
       </c>
       <c r="E41">
@@ -1782,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2540,12 +2600,12 @@
         <v>2.8000000000000003E-4</v>
       </c>
       <c r="D39" s="5">
-        <f>Phase1!C39</f>
-        <v>0.7</v>
+        <f>1.05*Phase1!C39</f>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
-        <v>0.2997200000000001</v>
+        <v>0.26472000000000007</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2560,12 +2620,12 @@
         <v>3.3600000000000004E-4</v>
       </c>
       <c r="D40" s="5">
-        <f>Phase1!C40</f>
-        <v>0.7</v>
+        <f>1.05*Phase1!C40</f>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>0.29966400000000004</v>
+        <v>0.26466400000000001</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2580,12 +2640,12 @@
         <v>4.8799999999999999E-4</v>
       </c>
       <c r="D41" s="5">
-        <f>Phase1!C41</f>
-        <v>0.7</v>
+        <f>1.05*Phase1!C41</f>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>0.299512</v>
+        <v>0.26451199999999997</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2618,7 +2678,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2667,12 +2727,12 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <f>15*B2</f>
-        <v>6.0000000000000001E-3</v>
+        <f>2*B2</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D2">
         <f>LN(C2/(1-C2))</f>
-        <v>-5.1099777374285189</v>
+        <v>-7.1300985101255776</v>
       </c>
       <c r="E2">
         <v>0.6</v>
@@ -2697,12 +2757,12 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C3">
-        <f>15*B3</f>
-        <v>6.0000000000000001E-3</v>
+        <f t="shared" ref="C3:C18" si="1">2*B3</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D3">
         <f>LN(C3/(1-C3))</f>
-        <v>-5.1099777374285189</v>
+        <v>-7.1300985101255776</v>
       </c>
       <c r="E3">
         <v>0.6</v>
@@ -2727,12 +2787,12 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C18" si="1">15*B4</f>
-        <v>7.4999999999999997E-3</v>
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">LN(C4/(1-C4))</f>
-        <v>-4.8853239920190807</v>
+        <v>-6.9067547786485539</v>
       </c>
       <c r="E4">
         <v>0.6</v>
@@ -2758,11 +2818,11 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-4.7014899569937691</v>
+        <v>-6.7242330016116636</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -2788,11 +2848,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1.0500000000000001E-2</v>
+        <v>1.4E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>-4.5458245078791428</v>
+        <v>-6.5698820614452957</v>
       </c>
       <c r="E6">
         <v>0.6</v>
@@ -2818,11 +2878,11 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>-4.4107760479598674</v>
+        <v>-6.4361503683694279</v>
       </c>
       <c r="E7">
         <v>0.6</v>
@@ -2848,11 +2908,11 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1.35E-2</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-4.2914736400182862</v>
+        <v>-6.3181669921333894</v>
       </c>
       <c r="E8">
         <v>0.6</v>
@@ -2878,11 +2938,11 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-4.1845914400698785</v>
+        <v>-6.2126060957515188</v>
       </c>
       <c r="E9">
         <v>0.6</v>
@@ -2908,11 +2968,11 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>2.7E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-3.5845472161816758</v>
+        <v>-5.6232149379259608</v>
       </c>
       <c r="E10">
         <v>0.6</v>
@@ -2938,11 +2998,11 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0.03</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-3.4760986898352733</v>
+        <v>-5.5174528964647074</v>
       </c>
       <c r="E11">
         <v>0.6</v>
@@ -2968,11 +3028,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-2.7515353130419489</v>
+        <v>-4.8202815656050371</v>
       </c>
       <c r="E12">
         <v>0.6</v>
@@ -2998,11 +3058,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-2.5123056239761148</v>
+        <v>-4.5951198501345898</v>
       </c>
       <c r="E13">
         <v>0.6</v>
@@ -3028,11 +3088,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.105</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-2.1428633681173319</v>
+        <v>-4.2545990249873764</v>
       </c>
       <c r="E14">
         <v>0.6</v>
@@ -3058,11 +3118,11 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.12</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-1.9924301646902063</v>
+        <v>-4.1190371748124717</v>
       </c>
       <c r="E15">
         <v>0.6</v>
@@ -3088,11 +3148,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>1.35E-2</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-4.2914736400182862</v>
+        <v>-6.3181669921333894</v>
       </c>
       <c r="E16">
         <v>0.6</v>
@@ -3118,11 +3178,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.16499999999999998</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-1.621486250950275</v>
+        <v>-3.7944672166765017</v>
       </c>
       <c r="E17">
         <v>0.6</v>
@@ -3148,11 +3208,11 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.21</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-1.3249254147435987</v>
+        <v>-3.5471512942852352</v>
       </c>
       <c r="E18">
         <v>0.6</v>
@@ -3180,7 +3240,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5319,6 +5379,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5543,16 +5612,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5569,12 +5637,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Wrote functions to analyze the data. Will eventually need to add in functions to analyze the crude risk associated with each estimator. However, not focusing on that yet.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78523F-5C68-FF4D-91B1-4654C414C82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CC7A67-A227-8A41-9B3A-4712421F1C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -86,7 +86,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Previously 0 because got confused on gw from conception and from LMP</t>
+    Previously 0 because got confused on gw from conception and from LMP
+Reply:
+    Increasing slightly so that we can increase the number of participants in the sample for now. Previously 0.1.</t>
       </text>
     </comment>
     <comment ref="E5" authorId="4" shapeId="0" xr:uid="{A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}">
@@ -94,7 +96,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Previously 0 because got confused on gw from conception and from LMP</t>
+    Previously 0 because got confused on gw from conception and from LMP
+Reply:
+    Increased slightly to increase # of participants. From 0.2 to 0.3</t>
       </text>
     </comment>
     <comment ref="E20" authorId="5" shapeId="0" xr:uid="{E0F99EF9-03C3-8340-B100-DF68AE4D4DF8}">
@@ -510,7 +514,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -538,12 +542,6 @@
       <color rgb="FF212121"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -915,8 +913,14 @@
   <threadedComment ref="E4" dT="2023-12-15T18:58:17.41" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{136807CB-0C11-AF4B-B455-BA7E6BADFC55}">
     <text>Previously 0 because got confused on gw from conception and from LMP</text>
   </threadedComment>
+  <threadedComment ref="E4" dT="2024-01-02T16:11:10.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{3D49A58A-FD00-2148-8526-B40661E9E107}" parentId="{136807CB-0C11-AF4B-B455-BA7E6BADFC55}">
+    <text>Increasing slightly so that we can increase the number of participants in the sample for now. Previously 0.1.</text>
+  </threadedComment>
   <threadedComment ref="E5" dT="2023-12-15T18:58:17.41" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}">
     <text>Previously 0 because got confused on gw from conception and from LMP</text>
+  </threadedComment>
+  <threadedComment ref="E5" dT="2024-01-02T16:11:31.32" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{ACF83317-8955-5743-AA16-ADD357B2BB13}" parentId="{A72EBEFA-8135-284E-ADA0-30EDB9DF31E0}">
+    <text>Increased slightly to increase # of participants. From 0.2 to 0.3</text>
   </threadedComment>
   <threadedComment ref="E20" dT="2023-12-15T18:59:01.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E0F99EF9-03C3-8340-B100-DF68AE4D4DF8}">
     <text xml:space="preserve">Previously 0.5. However, increased it to 1 because this is 20 gw from LMP. </text>
@@ -1058,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,7 +1144,7 @@
         <v>0.9</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1158,7 +1162,7 @@
         <v>0.9</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1176,7 +1180,7 @@
         <v>0.95</v>
       </c>
       <c r="E6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1190,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>1-B7-C7</f>
+        <f t="shared" ref="D7:D41" si="0">1-B7-C7</f>
         <v>0.95</v>
       </c>
       <c r="E7">
@@ -1208,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>1-B8-C8</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E8">
@@ -1226,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>1-B9-C9</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E9">
@@ -1244,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>1-B10-C10</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E10">
@@ -1262,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>1-B11-C11</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E11">
@@ -1280,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>1-B12-C12</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E12">
@@ -1298,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>1-B13-C13</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
       <c r="E13">
@@ -1316,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>1-B14-C14</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E14">
@@ -1334,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f>1-B15-C15</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E15">
@@ -1352,14 +1356,14 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>1-B16-C16</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1370,14 +1374,14 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>1-B17-C17</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1388,14 +1392,14 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f>1-B18-C18</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1406,14 +1410,14 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f>1-B19-C19</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E19">
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1424,14 +1428,14 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <f>1-B20-C20</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1442,14 +1446,14 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f>1-B21-C21</f>
+        <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1460,14 +1464,14 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <f>1-B22-C22</f>
+        <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1478,14 +1482,14 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <f>1-B23-C23</f>
+        <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1496,14 +1500,14 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f>1-B24-C24</f>
+        <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1514,18 +1518,14 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f>1-B25-C25</f>
+        <f t="shared" si="0"/>
         <v>0.997</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <f>0.8*C26</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1536,14 +1536,14 @@
         <v>0.01</v>
       </c>
       <c r="D26">
-        <f>1-B26-C26</f>
+        <f t="shared" si="0"/>
         <v>0.98699999999999999</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1554,14 +1554,14 @@
         <v>0.01</v>
       </c>
       <c r="D27">
-        <f>1-B27-C27</f>
+        <f t="shared" si="0"/>
         <v>0.98699999999999999</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1572,14 +1572,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D28">
-        <f>1-B28-C28</f>
+        <f t="shared" si="0"/>
         <v>0.98199999999999998</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1590,14 +1590,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29">
-        <f>1-B29-C29</f>
+        <f t="shared" si="0"/>
         <v>0.98199999999999998</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1608,14 +1608,14 @@
         <v>0.02</v>
       </c>
       <c r="D30">
-        <f>1-B30-C30</f>
+        <f t="shared" si="0"/>
         <v>0.97699999999999998</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1626,14 +1626,14 @@
         <v>0.02</v>
       </c>
       <c r="D31">
-        <f>1-B31-C31</f>
+        <f t="shared" si="0"/>
         <v>0.97699999999999998</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D32">
-        <f>1-B32-C32</f>
+        <f t="shared" si="0"/>
         <v>0.97199999999999998</v>
       </c>
       <c r="E32">
@@ -1662,7 +1662,7 @@
         <v>0.03</v>
       </c>
       <c r="D33">
-        <f>1-B33-C33</f>
+        <f t="shared" si="0"/>
         <v>0.96699999999999997</v>
       </c>
       <c r="E33">
@@ -1680,7 +1680,7 @@
         <v>0.09</v>
       </c>
       <c r="D34">
-        <f>1-B34-C34</f>
+        <f t="shared" si="0"/>
         <v>0.90700000000000003</v>
       </c>
       <c r="E34">
@@ -1698,7 +1698,7 @@
         <v>0.09</v>
       </c>
       <c r="D35">
-        <f>1-B35-C35</f>
+        <f t="shared" si="0"/>
         <v>0.90700000000000003</v>
       </c>
       <c r="E35">
@@ -1716,7 +1716,7 @@
         <v>0.09</v>
       </c>
       <c r="D36">
-        <f>1-B36-C36</f>
+        <f t="shared" si="0"/>
         <v>0.90700000000000003</v>
       </c>
       <c r="E36">
@@ -1735,7 +1735,7 @@
         <v>0.3</v>
       </c>
       <c r="D37">
-        <f>1-B37-C37</f>
+        <f t="shared" si="0"/>
         <v>0.69978999999999991</v>
       </c>
       <c r="E37">
@@ -1753,7 +1753,7 @@
         <v>0.35</v>
       </c>
       <c r="D38">
-        <f>1-B38-C38</f>
+        <f t="shared" si="0"/>
         <v>0.64973000000000003</v>
       </c>
       <c r="E38">
@@ -1771,7 +1771,7 @@
         <v>0.7</v>
       </c>
       <c r="D39">
-        <f>1-B39-C39</f>
+        <f t="shared" si="0"/>
         <v>0.29965000000000008</v>
       </c>
       <c r="E39">
@@ -1789,7 +1789,7 @@
         <v>0.7</v>
       </c>
       <c r="D40">
-        <f>1-B40-C40</f>
+        <f t="shared" si="0"/>
         <v>0.29958000000000007</v>
       </c>
       <c r="E40">
@@ -1807,7 +1807,7 @@
         <v>0.7</v>
       </c>
       <c r="D41">
-        <f>1-B41-C41</f>
+        <f t="shared" si="0"/>
         <v>0.29939000000000004</v>
       </c>
       <c r="E41">
@@ -1840,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2153,7 +2153,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2266,12 +2266,8 @@
         <f t="shared" si="2"/>
         <v>0.99760000000000004</v>
       </c>
-      <c r="L22">
-        <f>1/0.8</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2290,7 +2286,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2309,7 +2305,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2328,7 +2324,7 @@
         <v>0.99760000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2348,7 +2344,7 @@
         <v>0.99060000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2368,7 +2364,7 @@
         <v>0.99060000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2388,7 +2384,7 @@
         <v>0.98710000000000009</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2408,7 +2404,7 @@
         <v>0.98710000000000009</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2428,7 +2424,7 @@
         <v>0.98360000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2448,7 +2444,7 @@
         <v>0.98360000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2678,7 +2674,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2727,12 +2723,12 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <f>2*B2</f>
-        <v>8.0000000000000004E-4</v>
+        <f>10*B2</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D2">
         <f>LN(C2/(1-C2))</f>
-        <v>-7.1300985101255776</v>
+        <v>-5.5174528964647074</v>
       </c>
       <c r="E2">
         <v>0.6</v>
@@ -2757,12 +2753,12 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C18" si="1">2*B3</f>
-        <v>8.0000000000000004E-4</v>
+        <f t="shared" ref="C3:C18" si="1">10*B3</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D3">
         <f>LN(C3/(1-C3))</f>
-        <v>-7.1300985101255776</v>
+        <v>-5.5174528964647074</v>
       </c>
       <c r="E3">
         <v>0.6</v>
@@ -2788,11 +2784,11 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">LN(C4/(1-C4))</f>
-        <v>-6.9067547786485539</v>
+        <v>-5.2933048247244923</v>
       </c>
       <c r="E4">
         <v>0.6</v>
@@ -2818,11 +2814,11 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>1.1999999999999999E-3</v>
+        <v>5.9999999999999993E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-6.7242330016116636</v>
+        <v>-5.1099777374285189</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -2848,11 +2844,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1.4E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>-6.5698820614452957</v>
+        <v>-4.9548205149898594</v>
       </c>
       <c r="E6">
         <v>0.6</v>
@@ -2878,11 +2874,11 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1.6000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>-6.4361503683694279</v>
+        <v>-4.8202815656050371</v>
       </c>
       <c r="E7">
         <v>0.6</v>
@@ -2908,11 +2904,11 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1.8E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-6.3181669921333894</v>
+        <v>-4.7014899569937691</v>
       </c>
       <c r="E8">
         <v>0.6</v>
@@ -2938,11 +2934,11 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>2E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-6.2126060957515188</v>
+        <v>-4.5951198501345898</v>
       </c>
       <c r="E9">
         <v>0.6</v>
@@ -2968,11 +2964,11 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>3.5999999999999999E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-5.6232149379259608</v>
+        <v>-3.9992195504583012</v>
       </c>
       <c r="E10">
         <v>0.6</v>
@@ -2998,11 +2994,11 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>4.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-5.5174528964647074</v>
+        <v>-3.8918202981106265</v>
       </c>
       <c r="E11">
         <v>0.6</v>
@@ -3028,11 +3024,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>0.04</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-4.8202815656050371</v>
+        <v>-3.1780538303479453</v>
       </c>
       <c r="E12">
         <v>0.6</v>
@@ -3058,11 +3054,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-4.5951198501345898</v>
+        <v>-2.9444389791664403</v>
       </c>
       <c r="E13">
         <v>0.6</v>
@@ -3088,11 +3084,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-4.2545990249873764</v>
+        <v>-2.5866893440979424</v>
       </c>
       <c r="E14">
         <v>0.6</v>
@@ -3118,11 +3114,11 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-4.1190371748124717</v>
+        <v>-2.4423470353692043</v>
       </c>
       <c r="E15">
         <v>0.6</v>
@@ -3148,11 +3144,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>1.8E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-6.3181669921333894</v>
+        <v>-4.7014899569937691</v>
       </c>
       <c r="E16">
         <v>0.6</v>
@@ -3178,11 +3174,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>2.1999999999999999E-2</v>
+        <v>0.10999999999999999</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-3.7944672166765017</v>
+        <v>-2.0907410969337694</v>
       </c>
       <c r="E17">
         <v>0.6</v>
@@ -3208,11 +3204,11 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-3.5471512942852352</v>
+        <v>-1.8152899666382492</v>
       </c>
       <c r="E18">
         <v>0.6</v>
@@ -3240,7 +3236,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5379,15 +5375,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5612,15 +5599,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5637,4 +5625,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Simulated more cohorts of patients, for a total of 500 cohorts.
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CC7A67-A227-8A41-9B3A-4712421F1C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0203AF1-C8AB-394A-9C43-89B3E46E8648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -1842,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created parameter Excel files for each of the scenarios
</commit_message>
<xml_diff>
--- a/Simulation parameters.xlsx
+++ b/Simulation parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0203AF1-C8AB-394A-9C43-89B3E46E8648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86E6238-4A8B-084A-842B-D13CD3D2E5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="31800" yWindow="-280" windowWidth="28800" windowHeight="16180" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -605,9 +605,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -645,7 +645,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -751,7 +751,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -893,7 +893,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,7 +1144,7 @@
         <v>0.9</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>0.9</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
         <v>0.95</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1198,7 +1198,7 @@
         <v>0.95</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1216,7 +1216,7 @@
         <v>0.97</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>0.97</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1252,7 +1252,7 @@
         <v>0.97</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
         <v>0.97</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1288,7 +1288,7 @@
         <v>0.97</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>0.97</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
         <v>0.99</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1342,7 +1342,7 @@
         <v>0.99</v>
       </c>
       <c r="E15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>0.99</v>
       </c>
       <c r="E16">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1378,7 +1378,7 @@
         <v>0.99</v>
       </c>
       <c r="E17">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,7 +1396,7 @@
         <v>0.99</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>0.99</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1432,7 +1432,7 @@
         <v>0.99</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1842,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -5375,6 +5375,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5599,16 +5608,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5625,12 +5633,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>